<commit_message>
[fix bug khi .venv ko update .env ở ngoài]
fix lỗi API KEY của .venv KHÔNG KHỚP VỚI API key của .env ở ngoài => PHẢI TIẾN HÀNH: deactivate, xong activate lại mới load được .env ở ngoài
</commit_message>
<xml_diff>
--- a/5_TuningPrompting/output_data.xlsx
+++ b/5_TuningPrompting/output_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -529,16 +529,16 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>5.405269861221313</v>
+        <v>1.109622955322266</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>openai:gpt-4o-mini</t>
+          <t>groq:llama-3.3-70b-versatile</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -587,16 +587,276 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
+          <t>Hello.</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Request failed after 2 retries: Error code: 401 - {'error': {'message': 'Invalid API Key', 'type': 'invalid_request_error', 'code': 'invalid_api_key'}}</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr"/>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>openai:gpt-4o-mini</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>You are an assistant for teaching and learning English. Your task is to classify the intent of the user's utterance based on the intent list provided in the question
+&lt;task&gt;
+Step 1: Read the assistant's question and user's utterance.
+Step 2: Based on the information describing the customer's intent, determine which intent category the answer belongs to from the list below. If it doesn't match any intent, classify it as a "fallback" intent.
+Step 3: Return the intent name.
+&lt;/task&gt;
+&lt;tag&gt;
+## Descripble intent list
+[
+        {
+                "intent_name": "affirm_confirm",
+                "description": "Khách hàng nói xác nhận đúng khách hàng"
+        },
+        {
+                "intent_name": "absent",
+                "description": "Khách hàng nói đi vắng hoặc nghe hộ"
+        },
+        {
+                "intent_name": "deny_confirm",
+                "description": "Khách hàng xác nhận không phải khách hàng hoặc nhầm máy"
+        },
+        {
+                "intent_name": "busy",
+                "description": "khách hàng báo bận hoặc đang họp"
+        },
+        {
+                "intent_name": "cant_hear",
+                "description": "Khách hàng nói không nghe rõ"
+        },
+        {
+                "intent_name": "fallback",
+                "description": "Khách hàng nói những câu nói ngoài phạm vi không liên quan tới câu hỏi, nói tục hoặc chửi bậy"
+        }
+]
+&lt;/tag&gt;
+&lt;ouput&gt;
+The result should return only one intent that best matches the customer's response.
+The returned intent must belong to one of the intent lists mentioned above.
+Only the intent name should be generated, no other characters are allowed.
+&lt;/ouput&gt;</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
           <t>I eat breakfast.</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="E4" t="inlineStr">
         <is>
           <t>fallback</t>
         </is>
       </c>
-      <c r="F3" t="n">
-        <v>0.5770392417907715</v>
+      <c r="F4" t="n">
+        <v>0.6955010890960693</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr"/>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>groq:llama-3.3-70b-versatile</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>You are an assistant for teaching and learning English. Your task is to classify the intent of the user's utterance based on the intent list provided in the question
+&lt;task&gt;
+Step 1: Read the assistant's question and user's utterance.
+Step 2: Based on the information describing the customer's intent, determine which intent category the answer belongs to from the list below. If it doesn't match any intent, classify it as a "fallback" intent.
+Step 3: Return the intent name.
+&lt;/task&gt;
+&lt;tag&gt;
+## Descripble intent list
+[
+        {
+                "intent_name": "affirm_confirm",
+                "description": "Khách hàng nói xác nhận đúng khách hàng"
+        },
+        {
+                "intent_name": "absent",
+                "description": "Khách hàng nói đi vắng hoặc nghe hộ"
+        },
+        {
+                "intent_name": "deny_confirm",
+                "description": "Khách hàng xác nhận không phải khách hàng hoặc nhầm máy"
+        },
+        {
+                "intent_name": "busy",
+                "description": "khách hàng báo bận hoặc đang họp"
+        },
+        {
+                "intent_name": "cant_hear",
+                "description": "Khách hàng nói không nghe rõ"
+        },
+        {
+                "intent_name": "fallback",
+                "description": "Khách hàng nói những câu nói ngoài phạm vi không liên quan tới câu hỏi, nói tục hoặc chửi bậy"
+        }
+]
+&lt;/tag&gt;
+&lt;ouput&gt;
+The result should return only one intent that best matches the customer's response.
+The returned intent must belong to one of the intent lists mentioned above.
+Only the intent name should be generated, no other characters are allowed.
+&lt;/ouput&gt;</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>I eat breakfast.</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Request failed after 2 retries: Error code: 401 - {'error': {'message': 'Invalid API Key', 'type': 'invalid_request_error', 'code': 'invalid_api_key'}}</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr"/>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>openai:gpt-4o-mini</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>You are an assistant for teaching and learning English. Your task is to classify the intent of the user's utterance based on the intent list provided in the question
+&lt;task&gt;
+Step 1: Read the assistant's question and user's utterance.
+Step 2: Based on the information describing the customer's intent, determine which intent category the answer belongs to from the list below. If it doesn't match any intent, classify it as a "fallback" intent.
+Step 3: Return the intent name.
+&lt;/task&gt;
+&lt;tag&gt;
+## Descripble intent list
+[
+        {
+                "intent_name": "affirm_confirm",
+                "description": "Khách hàng nói xác nhận đúng khách hàng"
+        },
+        {
+                "intent_name": "absent",
+                "description": "Khách hàng nói đi vắng hoặc nghe hộ"
+        },
+        {
+                "intent_name": "deny_confirm",
+                "description": "Khách hàng xác nhận không phải khách hàng hoặc nhầm máy"
+        },
+        {
+                "intent_name": "busy",
+                "description": "khách hàng báo bận hoặc đang họp"
+        },
+        {
+                "intent_name": "cant_hear",
+                "description": "Khách hàng nói không nghe rõ"
+        },
+        {
+                "intent_name": "fallback",
+                "description": "Khách hàng nói những câu nói ngoài phạm vi không liên quan tới câu hỏi, nói tục hoặc chửi bậy"
+        }
+]
+&lt;/tag&gt;
+&lt;ouput&gt;
+The result should return only one intent that best matches the customer's response.
+The returned intent must belong to one of the intent lists mentioned above.
+Only the intent name should be generated, no other characters are allowed.
+&lt;/ouput&gt;</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>I eat breakfast.</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>fallback</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
+        <v>0.7523543834686279</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr"/>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>groq:llama-3.3-70b-versatile</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>You are an assistant for teaching and learning English. Your task is to classify the intent of the user's utterance based on the intent list provided in the question
+&lt;task&gt;
+Step 1: Read the assistant's question and user's utterance.
+Step 2: Based on the information describing the customer's intent, determine which intent category the answer belongs to from the list below. If it doesn't match any intent, classify it as a "fallback" intent.
+Step 3: Return the intent name.
+&lt;/task&gt;
+&lt;tag&gt;
+## Descripble intent list
+[
+        {
+                "intent_name": "affirm_confirm",
+                "description": "Khách hàng nói xác nhận đúng khách hàng"
+        },
+        {
+                "intent_name": "absent",
+                "description": "Khách hàng nói đi vắng hoặc nghe hộ"
+        },
+        {
+                "intent_name": "deny_confirm",
+                "description": "Khách hàng xác nhận không phải khách hàng hoặc nhầm máy"
+        },
+        {
+                "intent_name": "busy",
+                "description": "khách hàng báo bận hoặc đang họp"
+        },
+        {
+                "intent_name": "cant_hear",
+                "description": "Khách hàng nói không nghe rõ"
+        },
+        {
+                "intent_name": "fallback",
+                "description": "Khách hàng nói những câu nói ngoài phạm vi không liên quan tới câu hỏi, nói tục hoặc chửi bậy"
+        }
+]
+&lt;/tag&gt;
+&lt;ouput&gt;
+The result should return only one intent that best matches the customer's response.
+The returned intent must belong to one of the intent lists mentioned above.
+Only the intent name should be generated, no other characters are allowed.
+&lt;/ouput&gt;</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>I eat breakfast.</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Request failed after 2 retries: Error code: 401 - {'error': {'message': 'Invalid API Key', 'type': 'invalid_request_error', 'code': 'invalid_api_key'}}</t>
+        </is>
+      </c>
+      <c r="F7" t="n">
+        <v>-1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>